<commit_message>
update: belly width done
</commit_message>
<xml_diff>
--- a/data-result/flight-result-segment.xlsx
+++ b/data-result/flight-result-segment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyw/Documents/Chaper2/github-code/segmentation-3D/data-result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAA4E85-B25D-F940-9615-881C34CB59F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39AF10C-0A64-8747-9FA1-3CFC37DC3991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{1F2A6636-F2B4-D94A-95E1-54753800CFD8}"/>
+    <workbookView xWindow="14120" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{1F2A6636-F2B4-D94A-95E1-54753800CFD8}"/>
   </bookViews>
   <sheets>
     <sheet name="flights_sta" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3104" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3106" uniqueCount="489">
   <si>
     <t>velocity</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3306,6 +3306,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3333,32 +3357,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3366,11 +3366,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3868,7 +3868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C205A50B-3692-CE4C-9FBA-528FD68D4826}">
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="125" workbookViewId="0">
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
@@ -3898,23 +3898,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="191" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
-      <c r="F1" s="183"/>
-      <c r="G1" s="183"/>
-      <c r="H1" s="183"/>
-      <c r="I1" s="183"/>
-      <c r="J1" s="183"/>
-      <c r="K1" s="183"/>
-      <c r="L1" s="183"/>
-      <c r="M1" s="183"/>
-      <c r="N1" s="183"/>
-      <c r="O1" s="183"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
+      <c r="I1" s="191"/>
+      <c r="J1" s="191"/>
+      <c r="K1" s="191"/>
+      <c r="L1" s="191"/>
+      <c r="M1" s="191"/>
+      <c r="N1" s="191"/>
+      <c r="O1" s="191"/>
     </row>
     <row r="2" spans="1:24" ht="20">
       <c r="D2"/>
@@ -3927,20 +3927,20 @@
       <c r="W2" s="175"/>
     </row>
     <row r="3" spans="1:24" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="186" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="200" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="185" t="s">
+      <c r="C3" s="193" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="174" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="190"/>
-      <c r="F3" s="191"/>
+      <c r="E3" s="198"/>
+      <c r="F3" s="199"/>
       <c r="G3" s="174" t="s">
         <v>20</v>
       </c>
@@ -3948,16 +3948,16 @@
         <v>55</v>
       </c>
       <c r="I3" s="176"/>
-      <c r="J3" s="184" t="s">
+      <c r="J3" s="192" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="185"/>
-      <c r="L3" s="186"/>
-      <c r="M3" s="185" t="s">
+      <c r="K3" s="193"/>
+      <c r="L3" s="194"/>
+      <c r="M3" s="193" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="185"/>
-      <c r="O3" s="187"/>
+      <c r="N3" s="193"/>
+      <c r="O3" s="195"/>
       <c r="P3" s="174" t="s">
         <v>15</v>
       </c>
@@ -3967,20 +3967,20 @@
         <v>61</v>
       </c>
       <c r="T3" s="176"/>
-      <c r="U3" s="192" t="s">
+      <c r="U3" s="186" t="s">
         <v>57</v>
       </c>
-      <c r="V3" s="192" t="s">
+      <c r="V3" s="186" t="s">
         <v>60</v>
       </c>
-      <c r="W3" s="192" t="s">
+      <c r="W3" s="186" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:24" s="1" customFormat="1" ht="42" customHeight="1">
-      <c r="A4" s="189"/>
+      <c r="A4" s="197"/>
       <c r="B4" s="176"/>
-      <c r="C4" s="189"/>
+      <c r="C4" s="197"/>
       <c r="D4" s="3">
         <v>44935</v>
       </c>
@@ -3990,7 +3990,7 @@
       <c r="F4" s="155" t="s">
         <v>372</v>
       </c>
-      <c r="G4" s="188"/>
+      <c r="G4" s="196"/>
       <c r="H4" s="3" t="s">
         <v>53</v>
       </c>
@@ -4030,17 +4030,17 @@
       <c r="T4" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="U4" s="197" t="s">
+      <c r="U4" s="187" t="s">
         <v>57</v>
       </c>
-      <c r="V4" s="197"/>
-      <c r="W4" s="197"/>
+      <c r="V4" s="187"/>
+      <c r="W4" s="187"/>
     </row>
     <row r="5" spans="1:24">
       <c r="A5" s="87">
         <v>0.48541666666666666</v>
       </c>
-      <c r="B5" s="198">
+      <c r="B5" s="188">
         <v>8</v>
       </c>
       <c r="C5" s="29">
@@ -4106,7 +4106,7 @@
       <c r="A6" s="88">
         <v>0.47500000000000003</v>
       </c>
-      <c r="B6" s="199"/>
+      <c r="B6" s="189"/>
       <c r="C6" s="21">
         <v>1</v>
       </c>
@@ -4169,7 +4169,7 @@
       <c r="A7" s="87">
         <v>0.47847222222222219</v>
       </c>
-      <c r="B7" s="199"/>
+      <c r="B7" s="189"/>
       <c r="C7" s="8">
         <v>2</v>
       </c>
@@ -4233,7 +4233,7 @@
       <c r="A8" s="87">
         <v>0.48055555555555557</v>
       </c>
-      <c r="B8" s="199"/>
+      <c r="B8" s="189"/>
       <c r="C8" s="11">
         <v>3</v>
       </c>
@@ -4297,7 +4297,7 @@
       <c r="A9" s="87">
         <v>0.48333333333333334</v>
       </c>
-      <c r="B9" s="199"/>
+      <c r="B9" s="189"/>
       <c r="C9" s="8">
         <v>5</v>
       </c>
@@ -4357,7 +4357,7 @@
       <c r="A10" s="88">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B10" s="199"/>
+      <c r="B10" s="189"/>
       <c r="C10" s="8">
         <v>7</v>
       </c>
@@ -4420,7 +4420,7 @@
       <c r="A11" s="87">
         <v>0.56041666666666667</v>
       </c>
-      <c r="B11" s="199"/>
+      <c r="B11" s="189"/>
       <c r="C11" s="29">
         <v>7</v>
       </c>
@@ -4483,7 +4483,7 @@
       <c r="A12" s="88">
         <v>0.5541666666666667</v>
       </c>
-      <c r="B12" s="199"/>
+      <c r="B12" s="189"/>
       <c r="C12" s="11">
         <v>9</v>
       </c>
@@ -4546,7 +4546,7 @@
       <c r="A13" s="87">
         <v>0.55555555555555558</v>
       </c>
-      <c r="B13" s="200"/>
+      <c r="B13" s="190"/>
       <c r="C13" s="29">
         <v>9</v>
       </c>
@@ -4605,7 +4605,7 @@
       <c r="A14" s="87">
         <v>0.45277777777777778</v>
       </c>
-      <c r="B14" s="198">
+      <c r="B14" s="188">
         <v>10</v>
       </c>
       <c r="C14" s="29">
@@ -4670,7 +4670,7 @@
       <c r="A15" s="87">
         <v>0.46388888888888885</v>
       </c>
-      <c r="B15" s="199"/>
+      <c r="B15" s="189"/>
       <c r="C15" s="8">
         <v>2</v>
       </c>
@@ -4733,7 +4733,7 @@
       <c r="A16" s="87">
         <v>0.46597222222222223</v>
       </c>
-      <c r="B16" s="199"/>
+      <c r="B16" s="189"/>
       <c r="C16" s="8">
         <v>3</v>
       </c>
@@ -4798,7 +4798,7 @@
       <c r="A17" s="87">
         <v>0.46875</v>
       </c>
-      <c r="B17" s="199"/>
+      <c r="B17" s="189"/>
       <c r="C17" s="8">
         <v>5</v>
       </c>
@@ -4863,7 +4863,7 @@
       <c r="A18" s="88">
         <v>0.57638888888888895</v>
       </c>
-      <c r="B18" s="199"/>
+      <c r="B18" s="189"/>
       <c r="C18" s="8">
         <v>7</v>
       </c>
@@ -4928,7 +4928,7 @@
       <c r="A19" s="88">
         <v>0.57847222222222217</v>
       </c>
-      <c r="B19" s="200"/>
+      <c r="B19" s="190"/>
       <c r="C19" s="8">
         <v>9</v>
       </c>
@@ -4993,7 +4993,7 @@
       <c r="A20" s="87">
         <v>0.44930555555555557</v>
       </c>
-      <c r="B20" s="198">
+      <c r="B20" s="188">
         <v>15</v>
       </c>
       <c r="C20" s="8">
@@ -5060,7 +5060,7 @@
       <c r="A21" s="87">
         <v>0.44375000000000003</v>
       </c>
-      <c r="B21" s="199"/>
+      <c r="B21" s="189"/>
       <c r="C21" s="8">
         <v>1</v>
       </c>
@@ -5125,7 +5125,7 @@
       <c r="A22" s="87">
         <v>0.4381944444444445</v>
       </c>
-      <c r="B22" s="199"/>
+      <c r="B22" s="189"/>
       <c r="C22" s="8">
         <v>2</v>
       </c>
@@ -5190,7 +5190,7 @@
       <c r="A23" s="87">
         <v>0.44097222222222227</v>
       </c>
-      <c r="B23" s="199"/>
+      <c r="B23" s="189"/>
       <c r="C23" s="8">
         <v>3</v>
       </c>
@@ -5255,7 +5255,7 @@
       <c r="A24" s="87">
         <v>0.44305555555555554</v>
       </c>
-      <c r="B24" s="199"/>
+      <c r="B24" s="189"/>
       <c r="C24" s="8">
         <v>5</v>
       </c>
@@ -5320,7 +5320,7 @@
       <c r="A25" s="88">
         <v>0.58124999999999993</v>
       </c>
-      <c r="B25" s="199"/>
+      <c r="B25" s="189"/>
       <c r="C25" s="8">
         <v>7</v>
       </c>
@@ -5383,7 +5383,7 @@
       <c r="A26" s="88">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B26" s="200"/>
+      <c r="B26" s="190"/>
       <c r="C26" s="8">
         <v>9</v>
       </c>
@@ -6232,7 +6232,7 @@
       <c r="A39" s="162">
         <v>0.78194444444444444</v>
       </c>
-      <c r="B39" s="194">
+      <c r="B39" s="183">
         <v>8</v>
       </c>
       <c r="C39" s="147">
@@ -6291,7 +6291,7 @@
       <c r="A40" s="162">
         <v>0.78333333333333333</v>
       </c>
-      <c r="B40" s="195"/>
+      <c r="B40" s="184"/>
       <c r="C40" s="147">
         <v>5</v>
       </c>
@@ -6351,7 +6351,7 @@
       <c r="A41" s="162">
         <v>0.78680555555555554</v>
       </c>
-      <c r="B41" s="195"/>
+      <c r="B41" s="184"/>
       <c r="C41" s="147">
         <v>3</v>
       </c>
@@ -6407,7 +6407,7 @@
       <c r="A42" s="162">
         <v>0.78819444444444453</v>
       </c>
-      <c r="B42" s="195"/>
+      <c r="B42" s="184"/>
       <c r="C42" s="147">
         <v>5</v>
       </c>
@@ -6463,7 +6463,7 @@
       <c r="A43" s="162">
         <v>0.7895833333333333</v>
       </c>
-      <c r="B43" s="196">
+      <c r="B43" s="185">
         <v>15</v>
       </c>
       <c r="C43" s="147">
@@ -6518,7 +6518,7 @@
       <c r="A44" s="162">
         <v>0.79027777777777775</v>
       </c>
-      <c r="B44" s="196"/>
+      <c r="B44" s="185"/>
       <c r="C44" s="147">
         <v>5</v>
       </c>
@@ -6574,7 +6574,7 @@
       <c r="A45" s="162">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B45" s="196">
+      <c r="B45" s="185">
         <v>10</v>
       </c>
       <c r="C45" s="147">
@@ -6632,7 +6632,7 @@
       <c r="A46" s="162">
         <v>0.79305555555555562</v>
       </c>
-      <c r="B46" s="196"/>
+      <c r="B46" s="185"/>
       <c r="C46" s="147">
         <v>5</v>
       </c>
@@ -6690,7 +6690,7 @@
       <c r="A47" s="162">
         <v>0.7944444444444444</v>
       </c>
-      <c r="B47" s="196">
+      <c r="B47" s="185">
         <v>8</v>
       </c>
       <c r="C47" s="147">
@@ -6748,7 +6748,7 @@
       <c r="A48" s="162">
         <v>0.79583333333333339</v>
       </c>
-      <c r="B48" s="196"/>
+      <c r="B48" s="185"/>
       <c r="C48" s="147">
         <v>5</v>
       </c>
@@ -6855,6 +6855,15 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="B45:B46"/>
@@ -6870,15 +6879,6 @@
     <mergeCell ref="B20:B26"/>
     <mergeCell ref="B5:B13"/>
     <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6889,11 +6889,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F50920-10AA-FA43-834E-62930F0FDD71}">
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D382" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D388" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J393" sqref="J393:K395"/>
+      <selection pane="bottomRight" activeCell="H401" sqref="H401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6907,10 +6907,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="F1" s="203" t="s">
+      <c r="F1" s="204" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="203"/>
+      <c r="G1" s="204"/>
     </row>
     <row r="2" spans="1:13" ht="20">
       <c r="A2" s="3" t="s">
@@ -7025,7 +7025,7 @@
       <c r="H6" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I6" s="183" t="s">
+      <c r="I6" s="191" t="s">
         <v>112</v>
       </c>
     </row>
@@ -7046,7 +7046,7 @@
       <c r="H7" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I7" s="183"/>
+      <c r="I7" s="191"/>
       <c r="J7" s="2">
         <v>0.03</v>
       </c>
@@ -7075,9 +7075,9 @@
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="203"/>
-      <c r="B9" s="203"/>
-      <c r="C9" s="203"/>
+      <c r="A9" s="204"/>
+      <c r="B9" s="204"/>
+      <c r="C9" s="204"/>
       <c r="D9" s="27">
         <v>8</v>
       </c>
@@ -7246,7 +7246,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="202"/>
-      <c r="B18" s="203"/>
+      <c r="B18" s="204"/>
       <c r="C18" s="202"/>
       <c r="D18" s="2">
         <v>8</v>
@@ -7375,8 +7375,8 @@
       </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="203"/>
-      <c r="B25" s="203"/>
+      <c r="A25" s="204"/>
+      <c r="B25" s="204"/>
       <c r="C25" s="27" t="s">
         <v>116</v>
       </c>
@@ -7508,9 +7508,9 @@
       </c>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="203"/>
-      <c r="B31" s="203"/>
-      <c r="C31" s="203"/>
+      <c r="A31" s="204"/>
+      <c r="B31" s="204"/>
+      <c r="C31" s="204"/>
       <c r="D31" s="27">
         <v>6</v>
       </c>
@@ -7656,9 +7656,9 @@
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="203"/>
-      <c r="B39" s="203"/>
-      <c r="C39" s="203"/>
+      <c r="A39" s="204"/>
+      <c r="B39" s="204"/>
+      <c r="C39" s="204"/>
       <c r="D39" s="27">
         <v>11</v>
       </c>
@@ -7965,9 +7965,9 @@
       </c>
     </row>
     <row r="57" spans="1:14">
-      <c r="A57" s="203"/>
-      <c r="B57" s="203"/>
-      <c r="C57" s="203"/>
+      <c r="A57" s="204"/>
+      <c r="B57" s="204"/>
+      <c r="C57" s="204"/>
       <c r="D57" s="27">
         <v>9</v>
       </c>
@@ -8219,9 +8219,9 @@
       </c>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="203"/>
-      <c r="B72" s="203"/>
-      <c r="C72" s="203"/>
+      <c r="A72" s="204"/>
+      <c r="B72" s="204"/>
+      <c r="C72" s="204"/>
       <c r="D72" s="27">
         <v>14</v>
       </c>
@@ -8402,9 +8402,9 @@
       </c>
     </row>
     <row r="82" spans="1:13">
-      <c r="A82" s="203"/>
-      <c r="B82" s="203"/>
-      <c r="C82" s="203"/>
+      <c r="A82" s="204"/>
+      <c r="B82" s="204"/>
+      <c r="C82" s="204"/>
       <c r="D82" s="27">
         <v>8</v>
       </c>
@@ -8567,9 +8567,9 @@
       </c>
     </row>
     <row r="90" spans="1:13">
-      <c r="A90" s="203"/>
-      <c r="B90" s="203"/>
-      <c r="C90" s="203"/>
+      <c r="A90" s="204"/>
+      <c r="B90" s="204"/>
+      <c r="C90" s="204"/>
       <c r="D90" s="27">
         <v>8</v>
       </c>
@@ -8801,9 +8801,9 @@
       </c>
     </row>
     <row r="102" spans="1:13">
-      <c r="A102" s="203"/>
-      <c r="B102" s="203"/>
-      <c r="C102" s="203"/>
+      <c r="A102" s="204"/>
+      <c r="B102" s="204"/>
+      <c r="C102" s="204"/>
       <c r="D102" s="27">
         <v>7</v>
       </c>
@@ -9001,8 +9001,8 @@
       </c>
     </row>
     <row r="114" spans="1:14">
-      <c r="A114" s="203"/>
-      <c r="B114" s="203"/>
+      <c r="A114" s="204"/>
+      <c r="B114" s="204"/>
       <c r="C114" s="27" t="s">
         <v>116</v>
       </c>
@@ -9257,9 +9257,9 @@
       </c>
     </row>
     <row r="128" spans="1:14">
-      <c r="A128" s="203"/>
-      <c r="B128" s="203"/>
-      <c r="C128" s="203"/>
+      <c r="A128" s="204"/>
+      <c r="B128" s="204"/>
+      <c r="C128" s="204"/>
       <c r="D128" s="27">
         <v>4</v>
       </c>
@@ -9467,10 +9467,10 @@
       </c>
     </row>
     <row r="139" spans="1:14">
-      <c r="A139" s="203"/>
-      <c r="B139" s="203"/>
-      <c r="C139" s="203"/>
-      <c r="D139" s="203"/>
+      <c r="A139" s="204"/>
+      <c r="B139" s="204"/>
+      <c r="C139" s="204"/>
+      <c r="D139" s="204"/>
       <c r="E139" s="27">
         <v>1</v>
       </c>
@@ -9482,8 +9482,8 @@
       </c>
       <c r="H139" s="27"/>
       <c r="I139" s="57"/>
-      <c r="J139" s="203"/>
-      <c r="K139" s="203"/>
+      <c r="J139" s="204"/>
+      <c r="K139" s="204"/>
     </row>
     <row r="140" spans="1:14">
       <c r="A140" s="201">
@@ -9831,10 +9831,10 @@
       </c>
     </row>
     <row r="159" spans="1:11">
-      <c r="A159" s="203"/>
-      <c r="B159" s="203"/>
-      <c r="C159" s="203"/>
-      <c r="D159" s="203"/>
+      <c r="A159" s="204"/>
+      <c r="B159" s="204"/>
+      <c r="C159" s="204"/>
+      <c r="D159" s="204"/>
       <c r="E159" s="27">
         <v>1</v>
       </c>
@@ -10117,10 +10117,10 @@
       </c>
     </row>
     <row r="173" spans="1:14">
-      <c r="A173" s="203"/>
-      <c r="B173" s="203"/>
-      <c r="C173" s="203"/>
-      <c r="D173" s="203"/>
+      <c r="A173" s="204"/>
+      <c r="B173" s="204"/>
+      <c r="C173" s="204"/>
+      <c r="D173" s="204"/>
       <c r="E173" s="27">
         <v>1</v>
       </c>
@@ -10429,10 +10429,10 @@
       </c>
     </row>
     <row r="189" spans="1:14">
-      <c r="A189" s="203"/>
-      <c r="B189" s="203"/>
-      <c r="C189" s="203"/>
-      <c r="D189" s="203"/>
+      <c r="A189" s="204"/>
+      <c r="B189" s="204"/>
+      <c r="C189" s="204"/>
+      <c r="D189" s="204"/>
       <c r="E189" s="27">
         <v>1</v>
       </c>
@@ -10446,8 +10446,8 @@
       <c r="I189" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="J189" s="203"/>
-      <c r="K189" s="203">
+      <c r="J189" s="204"/>
+      <c r="K189" s="204">
         <v>3000</v>
       </c>
     </row>
@@ -10704,9 +10704,9 @@
       </c>
     </row>
     <row r="208" spans="1:13">
-      <c r="A208" s="203"/>
-      <c r="B208" s="203"/>
-      <c r="C208" s="203"/>
+      <c r="A208" s="204"/>
+      <c r="B208" s="204"/>
+      <c r="C208" s="204"/>
       <c r="D208" s="27">
         <v>20</v>
       </c>
@@ -11097,10 +11097,10 @@
       </c>
     </row>
     <row r="230" spans="1:13">
-      <c r="A230" s="203"/>
-      <c r="B230" s="203"/>
-      <c r="C230" s="203"/>
-      <c r="D230" s="203"/>
+      <c r="A230" s="204"/>
+      <c r="B230" s="204"/>
+      <c r="C230" s="204"/>
+      <c r="D230" s="204"/>
       <c r="E230" s="27">
         <v>1</v>
       </c>
@@ -11267,9 +11267,9 @@
       <c r="K238" s="202"/>
     </row>
     <row r="239" spans="1:13">
-      <c r="A239" s="203"/>
-      <c r="B239" s="203"/>
-      <c r="C239" s="203"/>
+      <c r="A239" s="204"/>
+      <c r="B239" s="204"/>
+      <c r="C239" s="204"/>
       <c r="D239" s="27">
         <v>10</v>
       </c>
@@ -11519,10 +11519,10 @@
       </c>
     </row>
     <row r="252" spans="1:11">
-      <c r="A252" s="203"/>
-      <c r="B252" s="203"/>
-      <c r="C252" s="203"/>
-      <c r="D252" s="203"/>
+      <c r="A252" s="204"/>
+      <c r="B252" s="204"/>
+      <c r="C252" s="204"/>
+      <c r="D252" s="204"/>
       <c r="E252" s="27">
         <v>1</v>
       </c>
@@ -11760,9 +11760,9 @@
       </c>
     </row>
     <row r="264" spans="1:14">
-      <c r="A264" s="203"/>
-      <c r="B264" s="203"/>
-      <c r="C264" s="203"/>
+      <c r="A264" s="204"/>
+      <c r="B264" s="204"/>
+      <c r="C264" s="204"/>
       <c r="D264" s="27">
         <v>12</v>
       </c>
@@ -11975,10 +11975,10 @@
       </c>
     </row>
     <row r="273" spans="1:14">
-      <c r="A273" s="203"/>
-      <c r="B273" s="203"/>
-      <c r="C273" s="203"/>
-      <c r="D273" s="203"/>
+      <c r="A273" s="204"/>
+      <c r="B273" s="204"/>
+      <c r="C273" s="204"/>
+      <c r="D273" s="204"/>
       <c r="E273" s="27">
         <v>1</v>
       </c>
@@ -12155,10 +12155,10 @@
       </c>
     </row>
     <row r="282" spans="1:14">
-      <c r="A282" s="203"/>
-      <c r="B282" s="203"/>
-      <c r="C282" s="203"/>
-      <c r="D282" s="203"/>
+      <c r="A282" s="204"/>
+      <c r="B282" s="204"/>
+      <c r="C282" s="204"/>
+      <c r="D282" s="204"/>
       <c r="E282" s="27">
         <v>1</v>
       </c>
@@ -12172,8 +12172,8 @@
         <v>168</v>
       </c>
       <c r="I282" s="57"/>
-      <c r="J282" s="203"/>
-      <c r="K282" s="203"/>
+      <c r="J282" s="204"/>
+      <c r="K282" s="204"/>
     </row>
     <row r="283" spans="1:14">
       <c r="A283" s="201">
@@ -12358,10 +12358,10 @@
       </c>
     </row>
     <row r="293" spans="1:14">
-      <c r="A293" s="203"/>
-      <c r="B293" s="203"/>
-      <c r="C293" s="203"/>
-      <c r="D293" s="203"/>
+      <c r="A293" s="204"/>
+      <c r="B293" s="204"/>
+      <c r="C293" s="204"/>
+      <c r="D293" s="204"/>
       <c r="E293" s="27">
         <v>1</v>
       </c>
@@ -12612,8 +12612,8 @@
       </c>
     </row>
     <row r="307" spans="1:14">
-      <c r="A307" s="203"/>
-      <c r="B307" s="203"/>
+      <c r="A307" s="204"/>
+      <c r="B307" s="204"/>
       <c r="C307" s="27" t="s">
         <v>116</v>
       </c>
@@ -12807,9 +12807,9 @@
       </c>
     </row>
     <row r="317" spans="1:14">
-      <c r="A317" s="203"/>
-      <c r="B317" s="203"/>
-      <c r="C317" s="203"/>
+      <c r="A317" s="204"/>
+      <c r="B317" s="204"/>
+      <c r="C317" s="204"/>
       <c r="D317" s="27">
         <v>9</v>
       </c>
@@ -13072,10 +13072,10 @@
       </c>
     </row>
     <row r="330" spans="1:14">
-      <c r="A330" s="203"/>
-      <c r="B330" s="203"/>
-      <c r="C330" s="203"/>
-      <c r="D330" s="203"/>
+      <c r="A330" s="204"/>
+      <c r="B330" s="204"/>
+      <c r="C330" s="204"/>
+      <c r="D330" s="204"/>
       <c r="E330" s="27">
         <v>2</v>
       </c>
@@ -13387,9 +13387,9 @@
       </c>
     </row>
     <row r="346" spans="1:14">
-      <c r="A346" s="203"/>
-      <c r="B346" s="203"/>
-      <c r="C346" s="203"/>
+      <c r="A346" s="204"/>
+      <c r="B346" s="204"/>
+      <c r="C346" s="204"/>
       <c r="D346" s="27">
         <v>12</v>
       </c>
@@ -13492,9 +13492,9 @@
       </c>
     </row>
     <row r="351" spans="1:14">
-      <c r="A351" s="203"/>
-      <c r="B351" s="203"/>
-      <c r="C351" s="203"/>
+      <c r="A351" s="204"/>
+      <c r="B351" s="204"/>
+      <c r="C351" s="204"/>
       <c r="D351" s="27">
         <v>5</v>
       </c>
@@ -13558,8 +13558,8 @@
       </c>
     </row>
     <row r="354" spans="1:17">
-      <c r="A354" s="203"/>
-      <c r="B354" s="203"/>
+      <c r="A354" s="204"/>
+      <c r="B354" s="204"/>
       <c r="C354" s="27" t="s">
         <v>116</v>
       </c>
@@ -13679,9 +13679,9 @@
       </c>
     </row>
     <row r="360" spans="1:17">
-      <c r="A360" s="203"/>
-      <c r="B360" s="203"/>
-      <c r="C360" s="203"/>
+      <c r="A360" s="204"/>
+      <c r="B360" s="204"/>
+      <c r="C360" s="204"/>
       <c r="D360" s="27">
         <v>3</v>
       </c>
@@ -13779,9 +13779,9 @@
       </c>
     </row>
     <row r="364" spans="1:17">
-      <c r="A364" s="203"/>
-      <c r="B364" s="203"/>
-      <c r="C364" s="203"/>
+      <c r="A364" s="204"/>
+      <c r="B364" s="204"/>
+      <c r="C364" s="204"/>
       <c r="D364" s="27">
         <v>1</v>
       </c>
@@ -14249,10 +14249,10 @@
       </c>
     </row>
     <row r="384" spans="1:19">
-      <c r="A384" s="204" t="s">
+      <c r="A384" s="203" t="s">
         <v>446</v>
       </c>
-      <c r="B384" s="204">
+      <c r="B384" s="203">
         <v>5</v>
       </c>
       <c r="C384" s="67" t="s">
@@ -14280,8 +14280,8 @@
       </c>
     </row>
     <row r="385" spans="1:20">
-      <c r="A385" s="183"/>
-      <c r="B385" s="183"/>
+      <c r="A385" s="191"/>
+      <c r="B385" s="191"/>
       <c r="C385" s="67" t="s">
         <v>115</v>
       </c>
@@ -14304,8 +14304,8 @@
       </c>
     </row>
     <row r="386" spans="1:20">
-      <c r="A386" s="183"/>
-      <c r="B386" s="183"/>
+      <c r="A386" s="191"/>
+      <c r="B386" s="191"/>
       <c r="C386" s="67" t="s">
         <v>115</v>
       </c>
@@ -14334,8 +14334,8 @@
       </c>
     </row>
     <row r="387" spans="1:20">
-      <c r="A387" s="183"/>
-      <c r="B387" s="183"/>
+      <c r="A387" s="191"/>
+      <c r="B387" s="191"/>
       <c r="C387" s="67" t="s">
         <v>115</v>
       </c>
@@ -14433,8 +14433,8 @@
       <c r="O390" s="171">
         <v>5</v>
       </c>
-      <c r="P390" s="6">
-        <v>1</v>
+      <c r="P390" s="6" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="391" spans="1:20">
@@ -15520,6 +15520,157 @@
     </row>
   </sheetData>
   <mergeCells count="175">
+    <mergeCell ref="C355:C357"/>
+    <mergeCell ref="D358:D359"/>
+    <mergeCell ref="C358:C360"/>
+    <mergeCell ref="A355:A360"/>
+    <mergeCell ref="D362:D363"/>
+    <mergeCell ref="C362:C364"/>
+    <mergeCell ref="A361:A364"/>
+    <mergeCell ref="A331:A346"/>
+    <mergeCell ref="C347:C348"/>
+    <mergeCell ref="C349:C351"/>
+    <mergeCell ref="A347:A351"/>
+    <mergeCell ref="C352:C353"/>
+    <mergeCell ref="A352:A354"/>
+    <mergeCell ref="C331:C336"/>
+    <mergeCell ref="B331:B346"/>
+    <mergeCell ref="B347:B351"/>
+    <mergeCell ref="B352:B354"/>
+    <mergeCell ref="B355:B360"/>
+    <mergeCell ref="B361:B364"/>
+    <mergeCell ref="J340:J341"/>
+    <mergeCell ref="D340:D341"/>
+    <mergeCell ref="K340:K341"/>
+    <mergeCell ref="K342:K343"/>
+    <mergeCell ref="J342:J343"/>
+    <mergeCell ref="D342:D343"/>
+    <mergeCell ref="C337:C346"/>
+    <mergeCell ref="C308:C313"/>
+    <mergeCell ref="C314:C317"/>
+    <mergeCell ref="A308:A317"/>
+    <mergeCell ref="C318:C324"/>
+    <mergeCell ref="D328:D330"/>
+    <mergeCell ref="C325:C330"/>
+    <mergeCell ref="A318:A330"/>
+    <mergeCell ref="A274:A282"/>
+    <mergeCell ref="C283:C290"/>
+    <mergeCell ref="D292:D293"/>
+    <mergeCell ref="C291:C293"/>
+    <mergeCell ref="A283:A293"/>
+    <mergeCell ref="C294:C306"/>
+    <mergeCell ref="A294:A307"/>
+    <mergeCell ref="C274:C278"/>
+    <mergeCell ref="B274:B282"/>
+    <mergeCell ref="B283:B293"/>
+    <mergeCell ref="B294:B307"/>
+    <mergeCell ref="B308:B317"/>
+    <mergeCell ref="B318:B330"/>
+    <mergeCell ref="D272:D273"/>
+    <mergeCell ref="D279:D280"/>
+    <mergeCell ref="D281:D282"/>
+    <mergeCell ref="J281:J282"/>
+    <mergeCell ref="K281:K282"/>
+    <mergeCell ref="C279:C282"/>
+    <mergeCell ref="C259:C264"/>
+    <mergeCell ref="A253:A264"/>
+    <mergeCell ref="C265:C266"/>
+    <mergeCell ref="D270:D271"/>
+    <mergeCell ref="C267:C273"/>
+    <mergeCell ref="A265:A273"/>
+    <mergeCell ref="B253:B264"/>
+    <mergeCell ref="B265:B273"/>
+    <mergeCell ref="C240:C246"/>
+    <mergeCell ref="D248:D249"/>
+    <mergeCell ref="D251:D252"/>
+    <mergeCell ref="C247:C252"/>
+    <mergeCell ref="A240:A252"/>
+    <mergeCell ref="C253:C258"/>
+    <mergeCell ref="C231:C236"/>
+    <mergeCell ref="D237:D238"/>
+    <mergeCell ref="J237:J238"/>
+    <mergeCell ref="B231:B239"/>
+    <mergeCell ref="B240:B252"/>
+    <mergeCell ref="K237:K238"/>
+    <mergeCell ref="C237:C239"/>
+    <mergeCell ref="A231:A239"/>
+    <mergeCell ref="C203:C208"/>
+    <mergeCell ref="A190:A208"/>
+    <mergeCell ref="C209:C226"/>
+    <mergeCell ref="D229:D230"/>
+    <mergeCell ref="C227:C230"/>
+    <mergeCell ref="A209:A230"/>
+    <mergeCell ref="B190:B208"/>
+    <mergeCell ref="B209:B230"/>
+    <mergeCell ref="D188:D189"/>
+    <mergeCell ref="J188:J189"/>
+    <mergeCell ref="K188:K189"/>
+    <mergeCell ref="C182:C189"/>
+    <mergeCell ref="A174:A189"/>
+    <mergeCell ref="C190:C202"/>
+    <mergeCell ref="C174:C181"/>
+    <mergeCell ref="D184:D185"/>
+    <mergeCell ref="D186:D187"/>
+    <mergeCell ref="J186:J187"/>
+    <mergeCell ref="K186:K187"/>
+    <mergeCell ref="B174:B189"/>
+    <mergeCell ref="B140:B159"/>
+    <mergeCell ref="J167:J169"/>
+    <mergeCell ref="K167:K169"/>
+    <mergeCell ref="D167:D169"/>
+    <mergeCell ref="C167:C173"/>
+    <mergeCell ref="D170:D171"/>
+    <mergeCell ref="D172:D173"/>
+    <mergeCell ref="D154:D155"/>
+    <mergeCell ref="D156:D157"/>
+    <mergeCell ref="D158:D159"/>
+    <mergeCell ref="C147:C159"/>
+    <mergeCell ref="J138:J139"/>
+    <mergeCell ref="K138:K139"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="A129:A139"/>
+    <mergeCell ref="J98:J99"/>
+    <mergeCell ref="K98:K99"/>
+    <mergeCell ref="C103:C113"/>
+    <mergeCell ref="A103:A114"/>
+    <mergeCell ref="C115:C126"/>
+    <mergeCell ref="B91:B102"/>
+    <mergeCell ref="B103:B114"/>
+    <mergeCell ref="C91:C97"/>
+    <mergeCell ref="D100:D101"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="A91:A102"/>
+    <mergeCell ref="C98:C102"/>
+    <mergeCell ref="C129:C137"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="A115:A128"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="B115:B128"/>
+    <mergeCell ref="B129:B139"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="A10:A18"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C83:C88"/>
+    <mergeCell ref="A83:A90"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="B10:B18"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="B32:B39"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="A40:A57"/>
+    <mergeCell ref="A58:A72"/>
+    <mergeCell ref="C58:C72"/>
+    <mergeCell ref="C73:C80"/>
+    <mergeCell ref="A73:A82"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="B58:B72"/>
     <mergeCell ref="A368:A371"/>
     <mergeCell ref="B368:B371"/>
     <mergeCell ref="A384:A388"/>
@@ -15544,157 +15695,6 @@
     <mergeCell ref="I150:I151"/>
     <mergeCell ref="D152:D153"/>
     <mergeCell ref="B160:B173"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="A10:A18"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C83:C88"/>
-    <mergeCell ref="A83:A90"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="B10:B18"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="B32:B39"/>
-    <mergeCell ref="C55:C57"/>
-    <mergeCell ref="A40:A57"/>
-    <mergeCell ref="A58:A72"/>
-    <mergeCell ref="C58:C72"/>
-    <mergeCell ref="C73:C80"/>
-    <mergeCell ref="A73:A82"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="B58:B72"/>
-    <mergeCell ref="J138:J139"/>
-    <mergeCell ref="K138:K139"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="A129:A139"/>
-    <mergeCell ref="J98:J99"/>
-    <mergeCell ref="K98:K99"/>
-    <mergeCell ref="C103:C113"/>
-    <mergeCell ref="A103:A114"/>
-    <mergeCell ref="C115:C126"/>
-    <mergeCell ref="B91:B102"/>
-    <mergeCell ref="B103:B114"/>
-    <mergeCell ref="C91:C97"/>
-    <mergeCell ref="D100:D101"/>
-    <mergeCell ref="D98:D99"/>
-    <mergeCell ref="A91:A102"/>
-    <mergeCell ref="C98:C102"/>
-    <mergeCell ref="C129:C137"/>
-    <mergeCell ref="C127:C128"/>
-    <mergeCell ref="A115:A128"/>
-    <mergeCell ref="D138:D139"/>
-    <mergeCell ref="B115:B128"/>
-    <mergeCell ref="B129:B139"/>
-    <mergeCell ref="B140:B159"/>
-    <mergeCell ref="J167:J169"/>
-    <mergeCell ref="K167:K169"/>
-    <mergeCell ref="D167:D169"/>
-    <mergeCell ref="C167:C173"/>
-    <mergeCell ref="D170:D171"/>
-    <mergeCell ref="D172:D173"/>
-    <mergeCell ref="D154:D155"/>
-    <mergeCell ref="D156:D157"/>
-    <mergeCell ref="D158:D159"/>
-    <mergeCell ref="C147:C159"/>
-    <mergeCell ref="D188:D189"/>
-    <mergeCell ref="J188:J189"/>
-    <mergeCell ref="K188:K189"/>
-    <mergeCell ref="C182:C189"/>
-    <mergeCell ref="A174:A189"/>
-    <mergeCell ref="C190:C202"/>
-    <mergeCell ref="C174:C181"/>
-    <mergeCell ref="D184:D185"/>
-    <mergeCell ref="D186:D187"/>
-    <mergeCell ref="J186:J187"/>
-    <mergeCell ref="K186:K187"/>
-    <mergeCell ref="B174:B189"/>
-    <mergeCell ref="K237:K238"/>
-    <mergeCell ref="C237:C239"/>
-    <mergeCell ref="A231:A239"/>
-    <mergeCell ref="C203:C208"/>
-    <mergeCell ref="A190:A208"/>
-    <mergeCell ref="C209:C226"/>
-    <mergeCell ref="D229:D230"/>
-    <mergeCell ref="C227:C230"/>
-    <mergeCell ref="A209:A230"/>
-    <mergeCell ref="B190:B208"/>
-    <mergeCell ref="B209:B230"/>
-    <mergeCell ref="C240:C246"/>
-    <mergeCell ref="D248:D249"/>
-    <mergeCell ref="D251:D252"/>
-    <mergeCell ref="C247:C252"/>
-    <mergeCell ref="A240:A252"/>
-    <mergeCell ref="C253:C258"/>
-    <mergeCell ref="C231:C236"/>
-    <mergeCell ref="D237:D238"/>
-    <mergeCell ref="J237:J238"/>
-    <mergeCell ref="B231:B239"/>
-    <mergeCell ref="B240:B252"/>
-    <mergeCell ref="D272:D273"/>
-    <mergeCell ref="D279:D280"/>
-    <mergeCell ref="D281:D282"/>
-    <mergeCell ref="J281:J282"/>
-    <mergeCell ref="K281:K282"/>
-    <mergeCell ref="C279:C282"/>
-    <mergeCell ref="C259:C264"/>
-    <mergeCell ref="A253:A264"/>
-    <mergeCell ref="C265:C266"/>
-    <mergeCell ref="D270:D271"/>
-    <mergeCell ref="C267:C273"/>
-    <mergeCell ref="A265:A273"/>
-    <mergeCell ref="B253:B264"/>
-    <mergeCell ref="B265:B273"/>
-    <mergeCell ref="A308:A317"/>
-    <mergeCell ref="C318:C324"/>
-    <mergeCell ref="D328:D330"/>
-    <mergeCell ref="C325:C330"/>
-    <mergeCell ref="A318:A330"/>
-    <mergeCell ref="A274:A282"/>
-    <mergeCell ref="C283:C290"/>
-    <mergeCell ref="D292:D293"/>
-    <mergeCell ref="C291:C293"/>
-    <mergeCell ref="A283:A293"/>
-    <mergeCell ref="C294:C306"/>
-    <mergeCell ref="A294:A307"/>
-    <mergeCell ref="C274:C278"/>
-    <mergeCell ref="B274:B282"/>
-    <mergeCell ref="B283:B293"/>
-    <mergeCell ref="B294:B307"/>
-    <mergeCell ref="B308:B317"/>
-    <mergeCell ref="B318:B330"/>
-    <mergeCell ref="J340:J341"/>
-    <mergeCell ref="D340:D341"/>
-    <mergeCell ref="K340:K341"/>
-    <mergeCell ref="K342:K343"/>
-    <mergeCell ref="J342:J343"/>
-    <mergeCell ref="D342:D343"/>
-    <mergeCell ref="C337:C346"/>
-    <mergeCell ref="C308:C313"/>
-    <mergeCell ref="C314:C317"/>
-    <mergeCell ref="C355:C357"/>
-    <mergeCell ref="D358:D359"/>
-    <mergeCell ref="C358:C360"/>
-    <mergeCell ref="A355:A360"/>
-    <mergeCell ref="D362:D363"/>
-    <mergeCell ref="C362:C364"/>
-    <mergeCell ref="A361:A364"/>
-    <mergeCell ref="A331:A346"/>
-    <mergeCell ref="C347:C348"/>
-    <mergeCell ref="C349:C351"/>
-    <mergeCell ref="A347:A351"/>
-    <mergeCell ref="C352:C353"/>
-    <mergeCell ref="A352:A354"/>
-    <mergeCell ref="C331:C336"/>
-    <mergeCell ref="B331:B346"/>
-    <mergeCell ref="B347:B351"/>
-    <mergeCell ref="B352:B354"/>
-    <mergeCell ref="B355:B360"/>
-    <mergeCell ref="B361:B364"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19517,7 +19517,7 @@
   <dimension ref="A1:S319"/>
   <sheetViews>
     <sheetView topLeftCell="A271" workbookViewId="0">
-      <selection activeCell="S294" sqref="S294"/>
+      <selection activeCell="J279" sqref="J279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19628,8 +19628,8 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="203"/>
-      <c r="B4" s="203"/>
+      <c r="A4" s="204"/>
+      <c r="B4" s="204"/>
       <c r="C4" s="2" t="s">
         <v>116</v>
       </c>
@@ -19982,8 +19982,8 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="203"/>
-      <c r="B17" s="203"/>
+      <c r="A17" s="204"/>
+      <c r="B17" s="204"/>
       <c r="C17" s="27" t="s">
         <v>116</v>
       </c>
@@ -20128,8 +20128,8 @@
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="203"/>
-      <c r="B22" s="203"/>
+      <c r="A22" s="204"/>
+      <c r="B22" s="204"/>
       <c r="C22" s="2" t="s">
         <v>116</v>
       </c>
@@ -20268,8 +20268,8 @@
       </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="203"/>
-      <c r="B27" s="203"/>
+      <c r="A27" s="204"/>
+      <c r="B27" s="204"/>
       <c r="C27" s="67" t="s">
         <v>115</v>
       </c>
@@ -20885,8 +20885,8 @@
       </c>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="203"/>
-      <c r="B50" s="203"/>
+      <c r="A50" s="204"/>
+      <c r="B50" s="204"/>
       <c r="C50" s="67" t="s">
         <v>115</v>
       </c>
@@ -21072,8 +21072,8 @@
       </c>
     </row>
     <row r="57" spans="1:12">
-      <c r="A57" s="203"/>
-      <c r="B57" s="203"/>
+      <c r="A57" s="204"/>
+      <c r="B57" s="204"/>
       <c r="C57" s="2" t="s">
         <v>116</v>
       </c>
@@ -21298,8 +21298,8 @@
       </c>
     </row>
     <row r="65" spans="1:12">
-      <c r="A65" s="203"/>
-      <c r="B65" s="203"/>
+      <c r="A65" s="204"/>
+      <c r="B65" s="204"/>
       <c r="C65" s="2" t="s">
         <v>116</v>
       </c>
@@ -21527,8 +21527,8 @@
       </c>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="203"/>
-      <c r="B73" s="203"/>
+      <c r="A73" s="204"/>
+      <c r="B73" s="204"/>
       <c r="C73" s="27" t="s">
         <v>116</v>
       </c>
@@ -21823,8 +21823,8 @@
       </c>
     </row>
     <row r="84" spans="1:12">
-      <c r="A84" s="203"/>
-      <c r="B84" s="203"/>
+      <c r="A84" s="204"/>
+      <c r="B84" s="204"/>
       <c r="C84" s="27" t="s">
         <v>116</v>
       </c>
@@ -22095,8 +22095,8 @@
       </c>
     </row>
     <row r="94" spans="1:12">
-      <c r="A94" s="203"/>
-      <c r="B94" s="203"/>
+      <c r="A94" s="204"/>
+      <c r="B94" s="204"/>
       <c r="C94" s="2" t="s">
         <v>116</v>
       </c>
@@ -22398,8 +22398,8 @@
       </c>
     </row>
     <row r="105" spans="1:12">
-      <c r="A105" s="203"/>
-      <c r="B105" s="203"/>
+      <c r="A105" s="204"/>
+      <c r="B105" s="204"/>
       <c r="C105" s="2" t="s">
         <v>116</v>
       </c>
@@ -22877,8 +22877,8 @@
       </c>
     </row>
     <row r="122" spans="1:12">
-      <c r="A122" s="203"/>
-      <c r="B122" s="203"/>
+      <c r="A122" s="204"/>
+      <c r="B122" s="204"/>
       <c r="C122" s="27" t="s">
         <v>116</v>
       </c>
@@ -23195,8 +23195,8 @@
       </c>
     </row>
     <row r="133" spans="1:12">
-      <c r="A133" s="203"/>
-      <c r="B133" s="203"/>
+      <c r="A133" s="204"/>
+      <c r="B133" s="204"/>
       <c r="C133" s="2" t="s">
         <v>116</v>
       </c>
@@ -23524,8 +23524,8 @@
       </c>
     </row>
     <row r="145" spans="1:12">
-      <c r="A145" s="203"/>
-      <c r="B145" s="203"/>
+      <c r="A145" s="204"/>
+      <c r="B145" s="204"/>
       <c r="C145" s="2" t="s">
         <v>116</v>
       </c>
@@ -24122,8 +24122,8 @@
       </c>
     </row>
     <row r="167" spans="1:12">
-      <c r="A167" s="203"/>
-      <c r="B167" s="203"/>
+      <c r="A167" s="204"/>
+      <c r="B167" s="204"/>
       <c r="C167" s="2" t="s">
         <v>116</v>
       </c>
@@ -24363,8 +24363,8 @@
       </c>
     </row>
     <row r="176" spans="1:12">
-      <c r="A176" s="203"/>
-      <c r="B176" s="203"/>
+      <c r="A176" s="204"/>
+      <c r="B176" s="204"/>
       <c r="C176" s="27" t="s">
         <v>116</v>
       </c>
@@ -24633,8 +24633,8 @@
       </c>
     </row>
     <row r="185" spans="1:12">
-      <c r="A185" s="203"/>
-      <c r="B185" s="203"/>
+      <c r="A185" s="204"/>
+      <c r="B185" s="204"/>
       <c r="C185" s="2" t="s">
         <v>116</v>
       </c>
@@ -25032,8 +25032,8 @@
       </c>
     </row>
     <row r="199" spans="1:12">
-      <c r="A199" s="203"/>
-      <c r="B199" s="203"/>
+      <c r="A199" s="204"/>
+      <c r="B199" s="204"/>
       <c r="C199" s="2" t="s">
         <v>116</v>
       </c>
@@ -25685,8 +25685,8 @@
       </c>
     </row>
     <row r="223" spans="1:12">
-      <c r="A223" s="203"/>
-      <c r="B223" s="203"/>
+      <c r="A223" s="204"/>
+      <c r="B223" s="204"/>
       <c r="C223" s="27" t="s">
         <v>116</v>
       </c>
@@ -26286,8 +26286,8 @@
       </c>
     </row>
     <row r="244" spans="1:12">
-      <c r="A244" s="203"/>
-      <c r="B244" s="203"/>
+      <c r="A244" s="204"/>
+      <c r="B244" s="204"/>
       <c r="C244" s="27" t="s">
         <v>116</v>
       </c>
@@ -26428,8 +26428,8 @@
       </c>
     </row>
     <row r="249" spans="1:12">
-      <c r="A249" s="203"/>
-      <c r="B249" s="203"/>
+      <c r="A249" s="204"/>
+      <c r="B249" s="204"/>
       <c r="C249" s="2" t="s">
         <v>116</v>
       </c>
@@ -26550,8 +26550,8 @@
       </c>
     </row>
     <row r="253" spans="1:12">
-      <c r="A253" s="203"/>
-      <c r="B253" s="203"/>
+      <c r="A253" s="204"/>
+      <c r="B253" s="204"/>
       <c r="C253" s="2" t="s">
         <v>116</v>
       </c>
@@ -26994,10 +26994,10 @@
       </c>
     </row>
     <row r="273" spans="1:19">
-      <c r="A273" s="204" t="s">
+      <c r="A273" s="203" t="s">
         <v>446</v>
       </c>
-      <c r="B273" s="204">
+      <c r="B273" s="203">
         <v>5</v>
       </c>
       <c r="C273" s="67" t="s">
@@ -27025,8 +27025,8 @@
       </c>
     </row>
     <row r="274" spans="1:19">
-      <c r="A274" s="183"/>
-      <c r="B274" s="183"/>
+      <c r="A274" s="191"/>
+      <c r="B274" s="191"/>
       <c r="C274" s="67" t="s">
         <v>115</v>
       </c>
@@ -27048,8 +27048,8 @@
       </c>
     </row>
     <row r="275" spans="1:19">
-      <c r="A275" s="183"/>
-      <c r="B275" s="183"/>
+      <c r="A275" s="191"/>
+      <c r="B275" s="191"/>
       <c r="C275" s="67" t="s">
         <v>115</v>
       </c>
@@ -27077,8 +27077,8 @@
       </c>
     </row>
     <row r="276" spans="1:19">
-      <c r="A276" s="183"/>
-      <c r="B276" s="183"/>
+      <c r="A276" s="191"/>
+      <c r="B276" s="191"/>
       <c r="C276" s="67" t="s">
         <v>115</v>
       </c>
@@ -27172,8 +27172,8 @@
       <c r="I279" s="171">
         <v>5</v>
       </c>
-      <c r="J279" s="171">
-        <v>1</v>
+      <c r="J279" s="171" t="s">
+        <v>469</v>
       </c>
       <c r="O279" t="s">
         <v>487</v>
@@ -28182,6 +28182,66 @@
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A28:A38"/>
+    <mergeCell ref="B28:B38"/>
+    <mergeCell ref="A39:A50"/>
+    <mergeCell ref="B39:B50"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="B51:B57"/>
+    <mergeCell ref="A58:A65"/>
+    <mergeCell ref="B58:B65"/>
+    <mergeCell ref="A66:A73"/>
+    <mergeCell ref="B66:B73"/>
+    <mergeCell ref="A74:A84"/>
+    <mergeCell ref="B74:B84"/>
+    <mergeCell ref="A85:A94"/>
+    <mergeCell ref="B85:B94"/>
+    <mergeCell ref="A95:A105"/>
+    <mergeCell ref="B95:B105"/>
+    <mergeCell ref="A106:A114"/>
+    <mergeCell ref="B106:B114"/>
+    <mergeCell ref="A115:A122"/>
+    <mergeCell ref="B115:B122"/>
+    <mergeCell ref="A123:A133"/>
+    <mergeCell ref="B123:B133"/>
+    <mergeCell ref="A134:A145"/>
+    <mergeCell ref="B134:B145"/>
+    <mergeCell ref="A146:A160"/>
+    <mergeCell ref="B146:B160"/>
+    <mergeCell ref="A161:A167"/>
+    <mergeCell ref="B161:B167"/>
+    <mergeCell ref="A168:A176"/>
+    <mergeCell ref="B168:B176"/>
+    <mergeCell ref="A177:A185"/>
+    <mergeCell ref="B177:B185"/>
+    <mergeCell ref="A186:A192"/>
+    <mergeCell ref="B186:B192"/>
+    <mergeCell ref="A193:A199"/>
+    <mergeCell ref="B193:B199"/>
+    <mergeCell ref="A200:A206"/>
+    <mergeCell ref="B200:B206"/>
+    <mergeCell ref="A207:A215"/>
+    <mergeCell ref="B207:B215"/>
+    <mergeCell ref="A216:A223"/>
+    <mergeCell ref="B216:B223"/>
+    <mergeCell ref="A224:A230"/>
+    <mergeCell ref="B224:B230"/>
+    <mergeCell ref="A231:A237"/>
+    <mergeCell ref="B231:B237"/>
+    <mergeCell ref="A238:A241"/>
+    <mergeCell ref="B238:B241"/>
+    <mergeCell ref="A242:A244"/>
+    <mergeCell ref="B242:B244"/>
     <mergeCell ref="A273:A277"/>
     <mergeCell ref="B273:B277"/>
     <mergeCell ref="A245:A249"/>
@@ -28190,66 +28250,6 @@
     <mergeCell ref="B250:B253"/>
     <mergeCell ref="A257:A260"/>
     <mergeCell ref="B257:B260"/>
-    <mergeCell ref="A231:A237"/>
-    <mergeCell ref="B231:B237"/>
-    <mergeCell ref="A238:A241"/>
-    <mergeCell ref="B238:B241"/>
-    <mergeCell ref="A242:A244"/>
-    <mergeCell ref="B242:B244"/>
-    <mergeCell ref="A207:A215"/>
-    <mergeCell ref="B207:B215"/>
-    <mergeCell ref="A216:A223"/>
-    <mergeCell ref="B216:B223"/>
-    <mergeCell ref="A224:A230"/>
-    <mergeCell ref="B224:B230"/>
-    <mergeCell ref="A186:A192"/>
-    <mergeCell ref="B186:B192"/>
-    <mergeCell ref="A193:A199"/>
-    <mergeCell ref="B193:B199"/>
-    <mergeCell ref="A200:A206"/>
-    <mergeCell ref="B200:B206"/>
-    <mergeCell ref="A161:A167"/>
-    <mergeCell ref="B161:B167"/>
-    <mergeCell ref="A168:A176"/>
-    <mergeCell ref="B168:B176"/>
-    <mergeCell ref="A177:A185"/>
-    <mergeCell ref="B177:B185"/>
-    <mergeCell ref="A123:A133"/>
-    <mergeCell ref="B123:B133"/>
-    <mergeCell ref="A134:A145"/>
-    <mergeCell ref="B134:B145"/>
-    <mergeCell ref="A146:A160"/>
-    <mergeCell ref="B146:B160"/>
-    <mergeCell ref="A95:A105"/>
-    <mergeCell ref="B95:B105"/>
-    <mergeCell ref="A106:A114"/>
-    <mergeCell ref="B106:B114"/>
-    <mergeCell ref="A115:A122"/>
-    <mergeCell ref="B115:B122"/>
-    <mergeCell ref="A66:A73"/>
-    <mergeCell ref="B66:B73"/>
-    <mergeCell ref="A74:A84"/>
-    <mergeCell ref="B74:B84"/>
-    <mergeCell ref="A85:A94"/>
-    <mergeCell ref="B85:B94"/>
-    <mergeCell ref="A39:A50"/>
-    <mergeCell ref="B39:B50"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="B51:B57"/>
-    <mergeCell ref="A58:A65"/>
-    <mergeCell ref="B58:B65"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A28:A38"/>
-    <mergeCell ref="B28:B38"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B12:B17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>